<commit_message>
Add Label to graphs
</commit_message>
<xml_diff>
--- a/function_2/steepest_descent_function_2_stepsize_0.001.xlsx
+++ b/function_2/steepest_descent_function_2_stepsize_0.001.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos\Steepest Descent\function_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2242D8-D5FE-4BB0-91D8-CC72A6DDAE7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31885F44-26AB-4059-B518-F0D432490D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4220,7 +4220,7 @@
                 </a:solidFill>
                 <a:effectLst/>
               </a:rPr>
-              <a:t>∇ f vs k</a:t>
+              <a:t>||∇ f || vs k</a:t>
             </a:r>
             <a:endParaRPr lang="es-GT" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>

</xml_diff>